<commit_message>
feat: :card_file_box: add new results
</commit_message>
<xml_diff>
--- a/zsceval/scripts/overcooked/eval/results/random3_m/bias/event_count_hsp.xlsx
+++ b/zsceval/scripts/overcooked/eval/results/random3_m/bias/event_count_hsp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BG46"/>
+  <dimension ref="A1:BG47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7887,55 +7887,55 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B42" t="n">
+        <v>0</v>
+      </c>
+      <c r="C42" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E42" t="n">
+        <v>7.09</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="I42" t="n">
+        <v>14.86</v>
+      </c>
+      <c r="J42" t="n">
         <v>0.03</v>
       </c>
-      <c r="C42" t="n">
-        <v>0</v>
-      </c>
-      <c r="D42" t="n">
-        <v>0</v>
-      </c>
-      <c r="E42" t="n">
-        <v>12.34</v>
-      </c>
-      <c r="F42" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="G42" t="n">
-        <v>12.93</v>
-      </c>
-      <c r="H42" t="n">
-        <v>0</v>
-      </c>
-      <c r="I42" t="n">
-        <v>0</v>
-      </c>
-      <c r="J42" t="n">
-        <v>0</v>
-      </c>
       <c r="K42" t="n">
-        <v>12.61</v>
+        <v>5.99</v>
       </c>
       <c r="L42" t="n">
-        <v>0</v>
+        <v>1.12</v>
       </c>
       <c r="M42" t="n">
-        <v>12.61</v>
+        <v>5.98</v>
       </c>
       <c r="N42" t="n">
-        <v>12.45</v>
+        <v>6</v>
       </c>
       <c r="O42" t="n">
-        <v>12.75</v>
+        <v>14.16</v>
       </c>
       <c r="P42" t="n">
-        <v>12.75</v>
+        <v>14.16</v>
       </c>
       <c r="Q42" t="n">
-        <v>12.75</v>
+        <v>14.16</v>
       </c>
       <c r="R42" t="n">
         <v>0</v>
@@ -7944,13 +7944,13 @@
         <v>0</v>
       </c>
       <c r="T42" t="n">
-        <v>12.75</v>
+        <v>0</v>
       </c>
       <c r="U42" t="n">
-        <v>0</v>
+        <v>14.16</v>
       </c>
       <c r="V42" t="n">
-        <v>12.76</v>
+        <v>6.97</v>
       </c>
       <c r="W42" t="n">
         <v>0</v>
@@ -7965,64 +7965,64 @@
         <v>0</v>
       </c>
       <c r="AA42" t="n">
-        <v>10.02</v>
+        <v>36.99</v>
       </c>
       <c r="AB42" t="n">
-        <v>307.59</v>
+        <v>302.58</v>
       </c>
       <c r="AC42" t="n">
-        <v>0.11</v>
+        <v>0.01</v>
       </c>
       <c r="AD42" t="n">
         <v>0</v>
       </c>
       <c r="AE42" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF42" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="AG42" t="n">
         <v>0.03</v>
       </c>
-      <c r="AF42" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG42" t="n">
-        <v>0</v>
-      </c>
       <c r="AH42" t="n">
-        <v>12.48</v>
+        <v>6.94</v>
       </c>
       <c r="AI42" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ42" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK42" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="AL42" t="n">
+        <v>14.82</v>
+      </c>
+      <c r="AM42" t="n">
         <v>0.03</v>
       </c>
-      <c r="AJ42" t="n">
-        <v>12.92</v>
-      </c>
-      <c r="AK42" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL42" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM42" t="n">
-        <v>0</v>
-      </c>
       <c r="AN42" t="n">
-        <v>12.75</v>
+        <v>5.96</v>
       </c>
       <c r="AO42" t="n">
-        <v>0</v>
+        <v>1.05</v>
       </c>
       <c r="AP42" t="n">
-        <v>12.75</v>
+        <v>5.96</v>
       </c>
       <c r="AQ42" t="n">
-        <v>12.61</v>
+        <v>5.96</v>
       </c>
       <c r="AR42" t="n">
-        <v>12.87</v>
+        <v>13.94</v>
       </c>
       <c r="AS42" t="n">
-        <v>12.87</v>
+        <v>13.94</v>
       </c>
       <c r="AT42" t="n">
-        <v>12.87</v>
+        <v>13.94</v>
       </c>
       <c r="AU42" t="n">
         <v>0</v>
@@ -8031,16 +8031,16 @@
         <v>0</v>
       </c>
       <c r="AW42" t="n">
-        <v>12.87</v>
+        <v>0</v>
       </c>
       <c r="AX42" t="n">
-        <v>0</v>
+        <v>13.94</v>
       </c>
       <c r="AY42" t="n">
-        <v>12.85</v>
+        <v>6.95</v>
       </c>
       <c r="AZ42" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="BA42" t="n">
         <v>0</v>
@@ -8049,16 +8049,16 @@
         <v>0</v>
       </c>
       <c r="BC42" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="BD42" t="n">
-        <v>11.69</v>
+        <v>37.02</v>
       </c>
       <c r="BE42" t="n">
-        <v>306.36</v>
+        <v>303.09</v>
       </c>
       <c r="BF42" t="n">
-        <v>0.15</v>
+        <v>0.91</v>
       </c>
       <c r="BG42" t="n">
         <v>0</v>
@@ -8066,13 +8066,13 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B43" t="n">
         <v>0</v>
       </c>
       <c r="C43" t="n">
-        <v>1.6</v>
+        <v>0.42</v>
       </c>
       <c r="D43" t="n">
         <v>0</v>
@@ -8087,10 +8087,10 @@
         <v>0</v>
       </c>
       <c r="H43" t="n">
-        <v>1.59</v>
+        <v>0.42</v>
       </c>
       <c r="I43" t="n">
-        <v>13.01</v>
+        <v>17</v>
       </c>
       <c r="J43" t="n">
         <v>0</v>
@@ -8108,13 +8108,13 @@
         <v>0</v>
       </c>
       <c r="O43" t="n">
-        <v>12.96</v>
+        <v>17</v>
       </c>
       <c r="P43" t="n">
-        <v>12.96</v>
+        <v>17</v>
       </c>
       <c r="Q43" t="n">
-        <v>12.96</v>
+        <v>17</v>
       </c>
       <c r="R43" t="n">
         <v>0</v>
@@ -8126,7 +8126,7 @@
         <v>0</v>
       </c>
       <c r="U43" t="n">
-        <v>12.96</v>
+        <v>17</v>
       </c>
       <c r="V43" t="n">
         <v>0</v>
@@ -8144,13 +8144,13 @@
         <v>0</v>
       </c>
       <c r="AA43" t="n">
-        <v>49.31</v>
+        <v>42.99</v>
       </c>
       <c r="AB43" t="n">
-        <v>321.52</v>
+        <v>322.17</v>
       </c>
       <c r="AC43" t="n">
-        <v>3.24</v>
+        <v>0.55</v>
       </c>
       <c r="AD43" t="n">
         <v>0</v>
@@ -8159,7 +8159,7 @@
         <v>0</v>
       </c>
       <c r="AF43" t="n">
-        <v>1.59</v>
+        <v>0.3</v>
       </c>
       <c r="AG43" t="n">
         <v>0</v>
@@ -8174,10 +8174,10 @@
         <v>0</v>
       </c>
       <c r="AK43" t="n">
-        <v>1.56</v>
+        <v>0.3</v>
       </c>
       <c r="AL43" t="n">
-        <v>13.03</v>
+        <v>17</v>
       </c>
       <c r="AM43" t="n">
         <v>0</v>
@@ -8195,13 +8195,13 @@
         <v>0</v>
       </c>
       <c r="AR43" t="n">
-        <v>12.99</v>
+        <v>17</v>
       </c>
       <c r="AS43" t="n">
-        <v>12.99</v>
+        <v>17</v>
       </c>
       <c r="AT43" t="n">
-        <v>12.99</v>
+        <v>17</v>
       </c>
       <c r="AU43" t="n">
         <v>0</v>
@@ -8213,7 +8213,7 @@
         <v>0</v>
       </c>
       <c r="AX43" t="n">
-        <v>12.99</v>
+        <v>17</v>
       </c>
       <c r="AY43" t="n">
         <v>0</v>
@@ -8231,13 +8231,13 @@
         <v>0</v>
       </c>
       <c r="BD43" t="n">
-        <v>47.37</v>
+        <v>44.21</v>
       </c>
       <c r="BE43" t="n">
-        <v>323.46</v>
+        <v>321.19</v>
       </c>
       <c r="BF43" t="n">
-        <v>3.55</v>
+        <v>0.61</v>
       </c>
       <c r="BG43" t="n">
         <v>0</v>
@@ -8245,13 +8245,13 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B44" t="n">
         <v>0</v>
       </c>
       <c r="C44" t="n">
-        <v>3.47</v>
+        <v>1.6</v>
       </c>
       <c r="D44" t="n">
         <v>0</v>
@@ -8266,10 +8266,10 @@
         <v>0</v>
       </c>
       <c r="H44" t="n">
-        <v>3.47</v>
+        <v>1.59</v>
       </c>
       <c r="I44" t="n">
-        <v>12.85</v>
+        <v>13.01</v>
       </c>
       <c r="J44" t="n">
         <v>0</v>
@@ -8287,13 +8287,13 @@
         <v>0</v>
       </c>
       <c r="O44" t="n">
-        <v>11.98</v>
+        <v>12.96</v>
       </c>
       <c r="P44" t="n">
-        <v>11.98</v>
+        <v>12.96</v>
       </c>
       <c r="Q44" t="n">
-        <v>11.98</v>
+        <v>12.96</v>
       </c>
       <c r="R44" t="n">
         <v>0</v>
@@ -8305,7 +8305,7 @@
         <v>0</v>
       </c>
       <c r="U44" t="n">
-        <v>11.98</v>
+        <v>12.96</v>
       </c>
       <c r="V44" t="n">
         <v>0</v>
@@ -8323,13 +8323,13 @@
         <v>0</v>
       </c>
       <c r="AA44" t="n">
-        <v>62.17</v>
+        <v>49.31</v>
       </c>
       <c r="AB44" t="n">
-        <v>305.97</v>
+        <v>321.52</v>
       </c>
       <c r="AC44" t="n">
-        <v>0.27</v>
+        <v>3.24</v>
       </c>
       <c r="AD44" t="n">
         <v>0</v>
@@ -8338,7 +8338,7 @@
         <v>0</v>
       </c>
       <c r="AF44" t="n">
-        <v>3.82</v>
+        <v>1.59</v>
       </c>
       <c r="AG44" t="n">
         <v>0</v>
@@ -8353,10 +8353,10 @@
         <v>0</v>
       </c>
       <c r="AK44" t="n">
-        <v>3.82</v>
+        <v>1.56</v>
       </c>
       <c r="AL44" t="n">
-        <v>12.84</v>
+        <v>13.03</v>
       </c>
       <c r="AM44" t="n">
         <v>0</v>
@@ -8374,13 +8374,13 @@
         <v>0</v>
       </c>
       <c r="AR44" t="n">
-        <v>12.03</v>
+        <v>12.99</v>
       </c>
       <c r="AS44" t="n">
-        <v>12.03</v>
+        <v>12.99</v>
       </c>
       <c r="AT44" t="n">
-        <v>12.03</v>
+        <v>12.99</v>
       </c>
       <c r="AU44" t="n">
         <v>0</v>
@@ -8392,7 +8392,7 @@
         <v>0</v>
       </c>
       <c r="AX44" t="n">
-        <v>12.03</v>
+        <v>12.99</v>
       </c>
       <c r="AY44" t="n">
         <v>0</v>
@@ -8410,13 +8410,13 @@
         <v>0</v>
       </c>
       <c r="BD44" t="n">
-        <v>62.26</v>
+        <v>47.37</v>
       </c>
       <c r="BE44" t="n">
-        <v>305.14</v>
+        <v>323.46</v>
       </c>
       <c r="BF44" t="n">
-        <v>0.21</v>
+        <v>3.55</v>
       </c>
       <c r="BG44" t="n">
         <v>0</v>
@@ -8424,55 +8424,55 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B45" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="C45" t="n">
-        <v>0</v>
+        <v>4.76</v>
       </c>
       <c r="D45" t="n">
         <v>0</v>
       </c>
       <c r="E45" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F45" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="G45" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="H45" t="n">
-        <v>0</v>
+        <v>4.76</v>
       </c>
       <c r="I45" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="J45" t="n">
         <v>0</v>
       </c>
       <c r="K45" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="L45" t="n">
         <v>0</v>
       </c>
       <c r="M45" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="N45" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="O45" t="n">
-        <v>16.93</v>
+        <v>13</v>
       </c>
       <c r="P45" t="n">
-        <v>16.93</v>
+        <v>13</v>
       </c>
       <c r="Q45" t="n">
-        <v>16.93</v>
+        <v>13</v>
       </c>
       <c r="R45" t="n">
         <v>0</v>
@@ -8481,13 +8481,13 @@
         <v>0</v>
       </c>
       <c r="T45" t="n">
-        <v>16.93</v>
+        <v>0</v>
       </c>
       <c r="U45" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="V45" t="n">
-        <v>16.87</v>
+        <v>0</v>
       </c>
       <c r="W45" t="n">
         <v>0</v>
@@ -8502,13 +8502,13 @@
         <v>0</v>
       </c>
       <c r="AA45" t="n">
-        <v>1</v>
+        <v>69.40000000000001</v>
       </c>
       <c r="AB45" t="n">
-        <v>300.18</v>
+        <v>295.02</v>
       </c>
       <c r="AC45" t="n">
-        <v>0.5600000000000001</v>
+        <v>1.32</v>
       </c>
       <c r="AD45" t="n">
         <v>0</v>
@@ -8517,49 +8517,49 @@
         <v>0</v>
       </c>
       <c r="AF45" t="n">
-        <v>0</v>
+        <v>4.78</v>
       </c>
       <c r="AG45" t="n">
         <v>0</v>
       </c>
       <c r="AH45" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="AI45" t="n">
         <v>0</v>
       </c>
       <c r="AJ45" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="AK45" t="n">
-        <v>0</v>
+        <v>4.77</v>
       </c>
       <c r="AL45" t="n">
-        <v>0</v>
+        <v>13.01</v>
       </c>
       <c r="AM45" t="n">
         <v>0</v>
       </c>
       <c r="AN45" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="AO45" t="n">
         <v>0</v>
       </c>
       <c r="AP45" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="AQ45" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="AR45" t="n">
-        <v>16.95</v>
+        <v>13</v>
       </c>
       <c r="AS45" t="n">
-        <v>16.95</v>
+        <v>13</v>
       </c>
       <c r="AT45" t="n">
-        <v>16.95</v>
+        <v>13</v>
       </c>
       <c r="AU45" t="n">
         <v>0</v>
@@ -8568,13 +8568,13 @@
         <v>0</v>
       </c>
       <c r="AW45" t="n">
-        <v>16.95</v>
+        <v>0</v>
       </c>
       <c r="AX45" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="AY45" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="AZ45" t="n">
         <v>0</v>
@@ -8589,13 +8589,13 @@
         <v>0</v>
       </c>
       <c r="BD45" t="n">
-        <v>0.98</v>
+        <v>68.95</v>
       </c>
       <c r="BE45" t="n">
-        <v>301.07</v>
+        <v>295.45</v>
       </c>
       <c r="BF45" t="n">
-        <v>0.66</v>
+        <v>1.48</v>
       </c>
       <c r="BG45" t="n">
         <v>0</v>
@@ -8603,10 +8603,10 @@
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B46" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
@@ -8615,10 +8615,10 @@
         <v>0</v>
       </c>
       <c r="E46" t="n">
-        <v>16.01</v>
+        <v>16</v>
       </c>
       <c r="F46" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="G46" t="n">
         <v>17</v>
@@ -8636,7 +8636,7 @@
         <v>16</v>
       </c>
       <c r="L46" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="M46" t="n">
         <v>16</v>
@@ -8645,13 +8645,13 @@
         <v>16</v>
       </c>
       <c r="O46" t="n">
-        <v>16.96</v>
+        <v>16.93</v>
       </c>
       <c r="P46" t="n">
-        <v>16.96</v>
+        <v>16.93</v>
       </c>
       <c r="Q46" t="n">
-        <v>16.96</v>
+        <v>16.93</v>
       </c>
       <c r="R46" t="n">
         <v>0</v>
@@ -8660,13 +8660,13 @@
         <v>0</v>
       </c>
       <c r="T46" t="n">
-        <v>16.96</v>
+        <v>16.93</v>
       </c>
       <c r="U46" t="n">
         <v>0</v>
       </c>
       <c r="V46" t="n">
-        <v>16.86</v>
+        <v>16.87</v>
       </c>
       <c r="W46" t="n">
         <v>0</v>
@@ -8681,19 +8681,19 @@
         <v>0</v>
       </c>
       <c r="AA46" t="n">
-        <v>2.26</v>
+        <v>1</v>
       </c>
       <c r="AB46" t="n">
-        <v>298.85</v>
+        <v>300.18</v>
       </c>
       <c r="AC46" t="n">
-        <v>0.06</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="AD46" t="n">
         <v>0</v>
       </c>
       <c r="AE46" t="n">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="AF46" t="n">
         <v>0</v>
@@ -8702,13 +8702,13 @@
         <v>0</v>
       </c>
       <c r="AH46" t="n">
-        <v>15.99</v>
+        <v>16</v>
       </c>
       <c r="AI46" t="n">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="AJ46" t="n">
-        <v>16.97</v>
+        <v>17</v>
       </c>
       <c r="AK46" t="n">
         <v>0</v>
@@ -8726,57 +8726,236 @@
         <v>0</v>
       </c>
       <c r="AP46" t="n">
+        <v>16</v>
+      </c>
+      <c r="AQ46" t="n">
+        <v>16</v>
+      </c>
+      <c r="AR46" t="n">
+        <v>16.95</v>
+      </c>
+      <c r="AS46" t="n">
+        <v>16.95</v>
+      </c>
+      <c r="AT46" t="n">
+        <v>16.95</v>
+      </c>
+      <c r="AU46" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV46" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW46" t="n">
+        <v>16.95</v>
+      </c>
+      <c r="AX46" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY46" t="n">
+        <v>16</v>
+      </c>
+      <c r="AZ46" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA46" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB46" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC46" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD46" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="BE46" t="n">
+        <v>301.07</v>
+      </c>
+      <c r="BF46" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="BG46" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B47" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" t="n">
+        <v>16.01</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="G47" t="n">
+        <v>17</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0</v>
+      </c>
+      <c r="J47" t="n">
+        <v>0</v>
+      </c>
+      <c r="K47" t="n">
+        <v>16</v>
+      </c>
+      <c r="L47" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M47" t="n">
+        <v>16</v>
+      </c>
+      <c r="N47" t="n">
+        <v>16</v>
+      </c>
+      <c r="O47" t="n">
+        <v>16.96</v>
+      </c>
+      <c r="P47" t="n">
+        <v>16.96</v>
+      </c>
+      <c r="Q47" t="n">
+        <v>16.96</v>
+      </c>
+      <c r="R47" t="n">
+        <v>0</v>
+      </c>
+      <c r="S47" t="n">
+        <v>0</v>
+      </c>
+      <c r="T47" t="n">
+        <v>16.96</v>
+      </c>
+      <c r="U47" t="n">
+        <v>0</v>
+      </c>
+      <c r="V47" t="n">
+        <v>16.86</v>
+      </c>
+      <c r="W47" t="n">
+        <v>0</v>
+      </c>
+      <c r="X47" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y47" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z47" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA47" t="n">
+        <v>2.26</v>
+      </c>
+      <c r="AB47" t="n">
+        <v>298.85</v>
+      </c>
+      <c r="AC47" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AD47" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE47" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AF47" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG47" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH47" t="n">
         <v>15.99</v>
       </c>
-      <c r="AQ46" t="n">
+      <c r="AI47" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AJ47" t="n">
+        <v>16.97</v>
+      </c>
+      <c r="AK47" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL47" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM47" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN47" t="n">
+        <v>16</v>
+      </c>
+      <c r="AO47" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP47" t="n">
         <v>15.99</v>
       </c>
-      <c r="AR46" t="n">
+      <c r="AQ47" t="n">
+        <v>15.99</v>
+      </c>
+      <c r="AR47" t="n">
         <v>16.57</v>
       </c>
-      <c r="AS46" t="n">
+      <c r="AS47" t="n">
         <v>16.57</v>
       </c>
-      <c r="AT46" t="n">
+      <c r="AT47" t="n">
         <v>16.57</v>
       </c>
-      <c r="AU46" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV46" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW46" t="n">
+      <c r="AU47" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV47" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW47" t="n">
         <v>16.57</v>
       </c>
-      <c r="AX46" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY46" t="n">
+      <c r="AX47" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY47" t="n">
         <v>15.99</v>
       </c>
-      <c r="AZ46" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA46" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB46" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC46" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD46" t="n">
+      <c r="AZ47" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA47" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB47" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC47" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD47" t="n">
         <v>2.44</v>
       </c>
-      <c r="BE46" t="n">
+      <c r="BE47" t="n">
         <v>299.73</v>
       </c>
-      <c r="BF46" t="n">
+      <c r="BF47" t="n">
         <v>0.02</v>
       </c>
-      <c r="BG46" t="n">
+      <c r="BG47" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>